<commit_message>
Vu Nguyen Edit UI
</commit_message>
<xml_diff>
--- a/documents/UI.xlsx
+++ b/documents/UI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="4" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>Mã bộ phận sử dụng</t>
   </si>
@@ -421,6 +421,12 @@
   </si>
   <si>
     <t>Các table còn lại làm tương tự</t>
+  </si>
+  <si>
+    <t>Không dùng cho module thêm</t>
+  </si>
+  <si>
+    <t>Giá trị lấy từ service</t>
   </si>
 </sst>
 </file>
@@ -823,8 +829,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
@@ -835,8 +841,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3590925" y="2066925"/>
-          <a:ext cx="714375" cy="266699"/>
+          <a:off x="4305300" y="2257425"/>
+          <a:ext cx="742950" cy="266699"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -905,40 +911,40 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="G22:G25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="G22:G25" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="G22:G25"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Ngân sách" dataDxfId="14"/>
+    <tableColumn id="1" name="Ngân sách" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table46" displayName="Table46" ref="H22:H25" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table46" displayName="Table46" ref="H22:H25" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="H22:H25"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Tự có" dataDxfId="11"/>
+    <tableColumn id="1" name="Tự có" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table467" displayName="Table467" ref="I22:I25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table467" displayName="Table467" ref="I22:I25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="I22:I25"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Liên doanh" dataDxfId="8"/>
+    <tableColumn id="1" name="Liên doanh" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table468" displayName="Table468" ref="J22:J25" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table468" displayName="Table468" ref="J22:J25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="J22:J25"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Khác" dataDxfId="5"/>
+    <tableColumn id="1" name="Khác" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1261,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -1410,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:N25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:L7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1668,9 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
+      <c r="L23" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
     </row>
@@ -1677,7 +1685,9 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
+      <c r="L24" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
     </row>
@@ -1698,15 +1708,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="6">
-    <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1715,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>